<commit_message>
switched rq 134 to distance-based instead of dre
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/Research/variables/Variable Definitions RQ134_PH1.xlsx
+++ b/dashboard-ui/src/components/Research/variables/Variable Definitions RQ134_PH1.xlsx
@@ -58,16 +58,16 @@
     <t>Target</t>
   </si>
   <si>
-    <t>Alignment score (ADM|target)</t>
-  </si>
-  <si>
-    <t>DRE Alignment score (ADM|target)</t>
-  </si>
-  <si>
-    <t>Alignment score (Delegator|target)</t>
-  </si>
-  <si>
-    <t>DRE Alignment score (Delegator|target)</t>
+    <t>P1E/Population Alignment score (ADM|target)</t>
+  </si>
+  <si>
+    <t>DRE/Distance Alignment score (ADM|target)</t>
+  </si>
+  <si>
+    <t>P1E/Population Alignment score (Delegator|target)</t>
+  </si>
+  <si>
+    <t>DRE/Distance Alignment score (Delegator|target)</t>
   </si>
   <si>
     <t>Alignment score (Participant_sim|Observed_ADM(target))</t>
@@ -88,10 +88,10 @@
     <t>Competence Error</t>
   </si>
   <si>
-    <t>Alignment score (Delegator|Observed_ADM (target))</t>
-  </si>
-  <si>
-    <t>DRE Alignment score (Delegator|Observed_ADM (target))</t>
+    <t>P1E/Population Alignment score (Delegator|Observed_ADM (target))</t>
+  </si>
+  <si>
+    <t>DRE/Distance Alignment score (Delegator|Observed_ADM (target))</t>
   </si>
   <si>
     <t>Truncation Error</t>
@@ -169,16 +169,16 @@
     <t>Target against which the presented ADM was run. For baseline ADMs, established a priori (most aligned). For aligned ADMs, determined by alignment with delegator text alignment scores</t>
   </si>
   <si>
-    <t>Calculated alignment score between the KDMA measurement of the ADM aligned to a particular target and that target from the Phase 1 Server</t>
-  </si>
-  <si>
-    <t>Calculated alignment score between the KDMA measurement of the ADM aligned to a particular target and that target from the DRE server for ADEPT, no change for ST</t>
-  </si>
-  <si>
-    <t>Calculated alignment score between the KDMA measurement of a delegator and a target from the Phase 1 server</t>
-  </si>
-  <si>
-    <t>Calculated alignment score between the KDMA measurement of a delegator and a target from the DRE server for ADEPT, no change for ST</t>
+    <t>Calculated alignment score between the KDMA measurement of the ADM aligned to a particular target and that target using the population-based endpoints</t>
+  </si>
+  <si>
+    <t>Calculated alignment score between the KDMA measurement of the ADM aligned to a particular target and that target using the distance-based endpoints in the Phase 1 server for ADEPT, no change for ST</t>
+  </si>
+  <si>
+    <t>Calculated alignment score between the KDMA measurement of a delegator and a target using the population-based endpoints</t>
+  </si>
+  <si>
+    <t>Calculated alignment score between the KDMA measurement of a delegator and a target using the distance-based endpoints in the Phase 1 server for ADEPT, no change for ST</t>
   </si>
   <si>
     <t>Compares the KDMA measurement based on participant probe responses in the simulated scenario to an ADM they observed in the delegation survey</t>
@@ -199,10 +199,10 @@
     <t>During the Phase 1 experiment, several ADMs had competence errors. This column shows which participants experienced one of those errors in the delegation survey</t>
   </si>
   <si>
-    <t>Compares the KDMA measurement based on delegator responses to the subset of probes from an ADM they observed in the delegation survey using the Phase 1 server and new endpoints</t>
-  </si>
-  <si>
-    <t>Compares the KDMA measurement based on delegator responses to the subset of probes from an ADM they observed in the delegation survey using the DRE server for ADEPT, no change for ST</t>
+    <t>Compares the KDMA measurement based on delegator responses to the subset of probes from an ADM they observed in the delegation survey using the Phase 1 server and new population-based endpoints</t>
+  </si>
+  <si>
+    <t>Compares the KDMA measurement based on delegator responses to the subset of probes from an ADM they observed in the delegation survey using the distance-based endpoints in the Phase 1 server for ADEPT, no change for ST</t>
   </si>
   <si>
     <t>During the January 2025 Evaluation, some ADMs had action text accidentally truncated. This column shows which participants experienced one of those errors and had their scores in the previous two columns (Alignment score (Delegator|Observed_ADM (target)), DRE Alignment score (Delegator|Observed_ADM (target))) fixed to omit the affected probe(s).</t>
@@ -285,13 +285,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -301,7 +307,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -336,16 +342,10 @@
   <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -353,8 +353,14 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,7 +671,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="17.290714285714284" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="18.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="19.290714285714284" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="6" width="19.576428571428572" customWidth="1" bestFit="1"/>
@@ -683,7 +689,7 @@
     <col min="17" max="17" style="6" width="32.57642857142857" customWidth="1" bestFit="1"/>
     <col min="18" max="18" style="6" width="32.57642857142857" customWidth="1" bestFit="1"/>
     <col min="19" max="19" style="6" width="46.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="6" width="27.005" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="7" width="27.005" customWidth="1" bestFit="1"/>
     <col min="21" max="21" style="6" width="47.71928571428572" customWidth="1" bestFit="1"/>
     <col min="22" max="22" style="6" width="22.576428571428572" customWidth="1" bestFit="1"/>
     <col min="23" max="23" style="6" width="21.719285714285714" customWidth="1" bestFit="1"/>
@@ -699,108 +705,108 @@
     <col min="33" max="33" style="6" width="19.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="28.5">
-      <c r="A1" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="30" customFormat="1" s="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="39.75" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="44.25" customFormat="1" s="1">
       <c r="A2" s="5" t="s">
         <v>33</v>
       </c>
@@ -879,7 +885,7 @@
       <c r="Z2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AA2" s="2" t="s">
         <v>34</v>
       </c>
       <c r="AB2" s="5" t="s">
@@ -901,7 +907,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="163.5" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="184.5" customFormat="1" s="1">
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
@@ -929,12 +935,12 @@
       <c r="I3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="2"/>
       <c r="K3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
       <c r="N3" s="5" t="s">
         <v>50</v>
       </c>
@@ -974,7 +980,7 @@
       <c r="Z3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AA3" s="2" t="s">
         <v>63</v>
       </c>
       <c r="AB3" s="5" t="s">
@@ -996,11 +1002,11 @@
         <v>64</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="253.5" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="299.25" customFormat="1" s="1">
       <c r="A4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="5" t="s">
         <v>68</v>
       </c>
@@ -1052,7 +1058,7 @@
       <c r="S4" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="T4" s="1"/>
+      <c r="T4" s="2"/>
       <c r="U4" s="5" t="s">
         <v>81</v>
       </c>
@@ -1071,7 +1077,7 @@
       <c r="Z4" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AA4" s="2" t="s">
         <v>84</v>
       </c>
       <c r="AB4" s="5" t="s">

</xml_diff>

<commit_message>
switched rq 134 to distance-based instead of dre (#277)
* switched rq 134 to distance-based instead of dre

* do not cache comparison data
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/Research/variables/Variable Definitions RQ134_PH1.xlsx
+++ b/dashboard-ui/src/components/Research/variables/Variable Definitions RQ134_PH1.xlsx
@@ -58,16 +58,16 @@
     <t>Target</t>
   </si>
   <si>
-    <t>Alignment score (ADM|target)</t>
-  </si>
-  <si>
-    <t>DRE Alignment score (ADM|target)</t>
-  </si>
-  <si>
-    <t>Alignment score (Delegator|target)</t>
-  </si>
-  <si>
-    <t>DRE Alignment score (Delegator|target)</t>
+    <t>P1E/Population Alignment score (ADM|target)</t>
+  </si>
+  <si>
+    <t>DRE/Distance Alignment score (ADM|target)</t>
+  </si>
+  <si>
+    <t>P1E/Population Alignment score (Delegator|target)</t>
+  </si>
+  <si>
+    <t>DRE/Distance Alignment score (Delegator|target)</t>
   </si>
   <si>
     <t>Alignment score (Participant_sim|Observed_ADM(target))</t>
@@ -88,10 +88,10 @@
     <t>Competence Error</t>
   </si>
   <si>
-    <t>Alignment score (Delegator|Observed_ADM (target))</t>
-  </si>
-  <si>
-    <t>DRE Alignment score (Delegator|Observed_ADM (target))</t>
+    <t>P1E/Population Alignment score (Delegator|Observed_ADM (target))</t>
+  </si>
+  <si>
+    <t>DRE/Distance Alignment score (Delegator|Observed_ADM (target))</t>
   </si>
   <si>
     <t>Truncation Error</t>
@@ -169,16 +169,16 @@
     <t>Target against which the presented ADM was run. For baseline ADMs, established a priori (most aligned). For aligned ADMs, determined by alignment with delegator text alignment scores</t>
   </si>
   <si>
-    <t>Calculated alignment score between the KDMA measurement of the ADM aligned to a particular target and that target from the Phase 1 Server</t>
-  </si>
-  <si>
-    <t>Calculated alignment score between the KDMA measurement of the ADM aligned to a particular target and that target from the DRE server for ADEPT, no change for ST</t>
-  </si>
-  <si>
-    <t>Calculated alignment score between the KDMA measurement of a delegator and a target from the Phase 1 server</t>
-  </si>
-  <si>
-    <t>Calculated alignment score between the KDMA measurement of a delegator and a target from the DRE server for ADEPT, no change for ST</t>
+    <t>Calculated alignment score between the KDMA measurement of the ADM aligned to a particular target and that target using the population-based endpoints</t>
+  </si>
+  <si>
+    <t>Calculated alignment score between the KDMA measurement of the ADM aligned to a particular target and that target using the distance-based endpoints in the Phase 1 server for ADEPT, no change for ST</t>
+  </si>
+  <si>
+    <t>Calculated alignment score between the KDMA measurement of a delegator and a target using the population-based endpoints</t>
+  </si>
+  <si>
+    <t>Calculated alignment score between the KDMA measurement of a delegator and a target using the distance-based endpoints in the Phase 1 server for ADEPT, no change for ST</t>
   </si>
   <si>
     <t>Compares the KDMA measurement based on participant probe responses in the simulated scenario to an ADM they observed in the delegation survey</t>
@@ -199,10 +199,10 @@
     <t>During the Phase 1 experiment, several ADMs had competence errors. This column shows which participants experienced one of those errors in the delegation survey</t>
   </si>
   <si>
-    <t>Compares the KDMA measurement based on delegator responses to the subset of probes from an ADM they observed in the delegation survey using the Phase 1 server and new endpoints</t>
-  </si>
-  <si>
-    <t>Compares the KDMA measurement based on delegator responses to the subset of probes from an ADM they observed in the delegation survey using the DRE server for ADEPT, no change for ST</t>
+    <t>Compares the KDMA measurement based on delegator responses to the subset of probes from an ADM they observed in the delegation survey using the Phase 1 server and new population-based endpoints</t>
+  </si>
+  <si>
+    <t>Compares the KDMA measurement based on delegator responses to the subset of probes from an ADM they observed in the delegation survey using the distance-based endpoints in the Phase 1 server for ADEPT, no change for ST</t>
   </si>
   <si>
     <t>During the January 2025 Evaluation, some ADMs had action text accidentally truncated. This column shows which participants experienced one of those errors and had their scores in the previous two columns (Alignment score (Delegator|Observed_ADM (target)), DRE Alignment score (Delegator|Observed_ADM (target))) fixed to omit the affected probe(s).</t>
@@ -285,13 +285,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -301,7 +307,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -336,16 +342,10 @@
   <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -353,8 +353,14 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,7 +671,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="17.290714285714284" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="18.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="19.290714285714284" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="6" width="19.576428571428572" customWidth="1" bestFit="1"/>
@@ -683,7 +689,7 @@
     <col min="17" max="17" style="6" width="32.57642857142857" customWidth="1" bestFit="1"/>
     <col min="18" max="18" style="6" width="32.57642857142857" customWidth="1" bestFit="1"/>
     <col min="19" max="19" style="6" width="46.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="6" width="27.005" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="7" width="27.005" customWidth="1" bestFit="1"/>
     <col min="21" max="21" style="6" width="47.71928571428572" customWidth="1" bestFit="1"/>
     <col min="22" max="22" style="6" width="22.576428571428572" customWidth="1" bestFit="1"/>
     <col min="23" max="23" style="6" width="21.719285714285714" customWidth="1" bestFit="1"/>
@@ -699,108 +705,108 @@
     <col min="33" max="33" style="6" width="19.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="28.5">
-      <c r="A1" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="30" customFormat="1" s="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="39.75" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="44.25" customFormat="1" s="1">
       <c r="A2" s="5" t="s">
         <v>33</v>
       </c>
@@ -879,7 +885,7 @@
       <c r="Z2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AA2" s="2" t="s">
         <v>34</v>
       </c>
       <c r="AB2" s="5" t="s">
@@ -901,7 +907,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="163.5" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="184.5" customFormat="1" s="1">
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
@@ -929,12 +935,12 @@
       <c r="I3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="2"/>
       <c r="K3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
       <c r="N3" s="5" t="s">
         <v>50</v>
       </c>
@@ -974,7 +980,7 @@
       <c r="Z3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AA3" s="2" t="s">
         <v>63</v>
       </c>
       <c r="AB3" s="5" t="s">
@@ -996,11 +1002,11 @@
         <v>64</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="253.5" customFormat="1" s="4">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="299.25" customFormat="1" s="1">
       <c r="A4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="5" t="s">
         <v>68</v>
       </c>
@@ -1052,7 +1058,7 @@
       <c r="S4" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="T4" s="1"/>
+      <c r="T4" s="2"/>
       <c r="U4" s="5" t="s">
         <v>81</v>
       </c>
@@ -1071,7 +1077,7 @@
       <c r="Z4" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AA4" s="2" t="s">
         <v>84</v>
       </c>
       <c r="AB4" s="5" t="s">

</xml_diff>